<commit_message>
add semesters divison and merging disciplines into common types
</commit_message>
<xml_diff>
--- a/PLVisualizerTest/TestDocxClient/LargeFileTest.xlsx
+++ b/PLVisualizerTest/TestDocxClient/LargeFileTest.xlsx
@@ -1,270 +1,421 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="42">
-  <si>
-    <t xml:space="preserve">Учебный период</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Подразделение</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Педагогическое задание</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дисциплина</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Виды учебной работы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Преподаватель</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAP-подразделение 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAP-подразделение 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Образовательные программы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Семестр 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Математико-механический факультет</t>
-  </si>
-  <si>
-    <t xml:space="preserve">058505 Учебная практика (научно-исследовательская работа)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Учебная практика (научно-исследовательская работа)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В присутствии преподавателя</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Литвинов Юрий Викторович</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кафедра системного программирования</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Факультет математико-механический</t>
-  </si>
-  <si>
-    <t xml:space="preserve">№5665,2021: Математическое обеспечение и администрирование информационных систем</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002212 Программирование</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Программирование</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Промежуточная аттестация (зач)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">№5162,2022: Технологии программирования</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002211 Информатика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Информатика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Промежуточная аттестация (экз)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Контрольные работы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Практические занятия</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Семинары</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Консультации</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Лабораторные работы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Лекции</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Семестр 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Семестр 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">№5162,2021: Технологии программирования</t>
-  </si>
-  <si>
-    <t xml:space="preserve">064792 Учебная практика 1 (научно-исследовательская работа)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Учебная практика 1 (научно-исследовательская работа)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Семестр 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">064851 Производственная практика (преддипломная)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Производственная практика (преддипломная)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кириленко Яков Александрович</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002187 Структуры и алгоритмы компьютерной обработки данных</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Структуры и алгоритмы компьютерной обработки данных</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="42">
+  <si>
+    <t>Учебный период</t>
+  </si>
+  <si>
+    <t>Подразделение</t>
+  </si>
+  <si>
+    <t>Педагогическое задание</t>
+  </si>
+  <si>
+    <t>Дисциплина</t>
+  </si>
+  <si>
+    <t>Виды учебной работы</t>
+  </si>
+  <si>
+    <t>Преподаватель</t>
+  </si>
+  <si>
+    <t>SAP-подразделение 2</t>
+  </si>
+  <si>
+    <t>SAP-подразделение 1</t>
+  </si>
+  <si>
+    <t>Образовательные программы</t>
+  </si>
+  <si>
+    <t>Семестр 1</t>
+  </si>
+  <si>
+    <t>Математико-механический факультет</t>
+  </si>
+  <si>
+    <t>058505 Учебная практика (научно-исследовательская работа)</t>
+  </si>
+  <si>
+    <t>Учебная практика (научно-исследовательская работа)</t>
+  </si>
+  <si>
+    <t>В присутствии преподавателя</t>
+  </si>
+  <si>
+    <t>Литвинов Юрий Викторович</t>
+  </si>
+  <si>
+    <t>Кафедра системного программирования</t>
+  </si>
+  <si>
+    <t>Факультет математико-механический</t>
+  </si>
+  <si>
+    <t>№5665,2021: Математическое обеспечение и администрирование информационных систем</t>
+  </si>
+  <si>
+    <t>002212 Программирование</t>
+  </si>
+  <si>
+    <t>Программирование</t>
+  </si>
+  <si>
+    <t>Промежуточная аттестация (зач)</t>
+  </si>
+  <si>
+    <t>№5162,2022: Технологии программирования</t>
+  </si>
+  <si>
+    <t>002211 Информатика</t>
+  </si>
+  <si>
+    <t>Информатика</t>
+  </si>
+  <si>
+    <t>Промежуточная аттестация (экз)</t>
+  </si>
+  <si>
+    <t>Контрольные работы</t>
+  </si>
+  <si>
+    <t>Практические занятия</t>
+  </si>
+  <si>
+    <t>Семинары</t>
+  </si>
+  <si>
+    <t>Консультации</t>
+  </si>
+  <si>
+    <t>Лабораторные работы</t>
+  </si>
+  <si>
+    <t>Лекции</t>
+  </si>
+  <si>
+    <t>Семестр 2</t>
+  </si>
+  <si>
+    <t>Семестр 3</t>
+  </si>
+  <si>
+    <t>№5162,2021: Технологии программирования</t>
+  </si>
+  <si>
+    <t>064792 Учебная практика 1 (научно-исследовательская работа)</t>
+  </si>
+  <si>
+    <t>Учебная практика 1 (научно-исследовательская работа)</t>
+  </si>
+  <si>
+    <t>Семестр 4</t>
+  </si>
+  <si>
+    <t>064851 Производственная практика (преддипломная)</t>
+  </si>
+  <si>
+    <t>Производственная практика (преддипломная)</t>
+  </si>
+  <si>
+    <t>Кириленко Яков Александрович</t>
+  </si>
+  <si>
+    <t>002187 Структуры и алгоритмы компьютерной обработки данных</t>
+  </si>
+  <si>
+    <t>Структуры и алгоритмы компьютерной обработки данных</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="3">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  </cellStyleXfs>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+  <a:themeElements>
+    <a:clrScheme name="Sheets">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4285F4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="EA4335"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="FBBC04"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="34A853"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="FF6D01"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="46BDC6"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="1155CC"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="1155CC"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Sheets">
+      <a:majorFont>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="80.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="69.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="49.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="46.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.77"/>
+    <col customWidth="1" min="2" max="2" width="30.13"/>
+    <col customWidth="1" min="3" max="3" width="51.75"/>
+    <col customWidth="1" min="4" max="4" width="45.75"/>
+    <col customWidth="1" min="5" max="5" width="26.5"/>
+    <col customWidth="1" min="6" max="6" width="25.88"/>
+    <col customWidth="1" min="7" max="7" width="32.5"/>
+    <col customWidth="1" min="8" max="8" width="29.75"/>
+    <col customWidth="1" min="9" max="9" width="72.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -293,14 +444,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -322,7 +473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -351,7 +502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -380,7 +531,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -409,7 +560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -438,7 +589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -467,7 +618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -496,7 +647,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -525,7 +676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -554,7 +705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -583,7 +734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -612,7 +763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -641,7 +792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -670,7 +821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -699,7 +850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -728,7 +879,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -757,7 +908,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -786,7 +937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -815,7 +966,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -844,7 +995,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -873,7 +1024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -902,7 +1053,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -931,7 +1082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -960,7 +1111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -989,7 +1140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -1018,7 +1169,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1047,7 +1198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1076,7 +1227,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1105,7 +1256,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1134,7 +1285,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1163,7 +1314,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -1192,7 +1343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -1221,7 +1372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1250,7 +1401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -1279,7 +1430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -1308,7 +1459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1337,13 +1488,326 @@
         <v>33</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wip api exceptions handling
</commit_message>
<xml_diff>
--- a/PLVisualizerTest/TestDocxClient/LargeFileTest.xlsx
+++ b/PLVisualizerTest/TestDocxClient/LargeFileTest.xlsx
@@ -55,7 +55,7 @@
     <t>В присутствии преподавателя</t>
   </si>
   <si>
-    <t>Литвинов Юрий Викторович</t>
+    <t>Литвинов Юрий Викторович, доцент</t>
   </si>
   <si>
     <t>Кафедра системного программирования</t>
@@ -130,7 +130,7 @@
     <t>Производственная практика (преддипломная)</t>
   </si>
   <si>
-    <t>Кириленко Яков Александрович</t>
+    <t>Кириленко Яков Александрович, старший преподаватель</t>
   </si>
   <si>
     <t>002187 Структуры и алгоритмы компьютерной обработки данных</t>
@@ -143,7 +143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -156,6 +156,10 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -179,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -188,6 +192,12 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,7 +419,7 @@
     <col customWidth="1" min="3" max="3" width="51.75"/>
     <col customWidth="1" min="4" max="4" width="45.75"/>
     <col customWidth="1" min="5" max="5" width="26.5"/>
-    <col customWidth="1" min="6" max="6" width="25.88"/>
+    <col customWidth="1" min="6" max="6" width="45.63"/>
     <col customWidth="1" min="7" max="7" width="32.5"/>
     <col customWidth="1" min="8" max="8" width="29.75"/>
     <col customWidth="1" min="9" max="9" width="72.63"/>
@@ -460,7 +470,7 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -489,7 +499,7 @@
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -518,7 +528,7 @@
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -547,7 +557,7 @@
       <c r="E5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -576,7 +586,7 @@
       <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -605,7 +615,7 @@
       <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -634,7 +644,7 @@
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -663,7 +673,7 @@
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -692,7 +702,7 @@
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -721,7 +731,7 @@
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -750,7 +760,7 @@
       <c r="E12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -779,7 +789,7 @@
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -808,7 +818,7 @@
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -837,7 +847,7 @@
       <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -866,7 +876,7 @@
       <c r="E16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -895,7 +905,7 @@
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -924,7 +934,7 @@
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -953,7 +963,7 @@
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -982,7 +992,7 @@
       <c r="E20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -1011,7 +1021,7 @@
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -1040,7 +1050,7 @@
       <c r="E22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1069,7 +1079,7 @@
       <c r="E23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -1098,7 +1108,7 @@
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -1127,7 +1137,7 @@
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -1156,7 +1166,7 @@
       <c r="E26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -1185,7 +1195,7 @@
       <c r="E27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -1214,7 +1224,7 @@
       <c r="E28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -1243,7 +1253,7 @@
       <c r="E29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -1272,7 +1282,7 @@
       <c r="E30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -1301,7 +1311,7 @@
       <c r="E31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -1330,7 +1340,7 @@
       <c r="E32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -1359,7 +1369,7 @@
       <c r="E33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -1388,7 +1398,7 @@
       <c r="E34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -1417,7 +1427,7 @@
       <c r="E35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G35" s="1" t="s">
@@ -1446,7 +1456,7 @@
       <c r="E36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -1475,7 +1485,7 @@
       <c r="E37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -1504,7 +1514,7 @@
       <c r="E38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -1533,7 +1543,7 @@
       <c r="E39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -1562,7 +1572,7 @@
       <c r="E40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -1591,7 +1601,7 @@
       <c r="E41" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="1" t="s">
@@ -1620,7 +1630,7 @@
       <c r="E42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="1" t="s">
@@ -1649,7 +1659,7 @@
       <c r="E43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
@@ -1678,7 +1688,7 @@
       <c r="E44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G44" s="1" t="s">
@@ -1707,7 +1717,7 @@
       <c r="E45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
@@ -1736,7 +1746,7 @@
       <c r="E46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
@@ -1765,7 +1775,7 @@
       <c r="E47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G47" s="1" t="s">
@@ -1794,7 +1804,7 @@
       <c r="E48" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G48" s="1" t="s">
@@ -1806,6 +1816,319 @@
       <c r="I48" s="1" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="49">
+      <c r="B49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51">
+      <c r="B51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54">
+      <c r="B54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61">
+      <c r="B61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62">
+      <c r="B62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63">
+      <c r="B63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64">
+      <c r="B64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66">
+      <c r="B66" s="1"/>
+      <c r="D66" s="4"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67">
+      <c r="B67" s="1"/>
+      <c r="D67" s="4"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68">
+      <c r="B68" s="1"/>
+      <c r="D68" s="4"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69">
+      <c r="B69" s="1"/>
+      <c r="D69" s="4"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70">
+      <c r="B70" s="1"/>
+      <c r="D70" s="4"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71">
+      <c r="B71" s="1"/>
+      <c r="D71" s="4"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72">
+      <c r="B72" s="1"/>
+      <c r="D72" s="4"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73">
+      <c r="B73" s="1"/>
+      <c r="D73" s="4"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="1"/>
+      <c r="D74" s="4"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="1"/>
+      <c r="D75" s="4"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76">
+      <c r="B76" s="1"/>
+      <c r="D76" s="4"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77">
+      <c r="B77" s="1"/>
+      <c r="D77" s="4"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="1"/>
+      <c r="D78" s="4"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="1"/>
+      <c r="D79" s="4"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80">
+      <c r="B80" s="1"/>
+      <c r="D80" s="4"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81">
+      <c r="B81" s="1"/>
+      <c r="D81" s="4"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82">
+      <c r="B82" s="1"/>
+      <c r="D82" s="4"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83">
+      <c r="B83" s="1"/>
+      <c r="D83" s="4"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84">
+      <c r="B84" s="1"/>
+      <c r="D84" s="4"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85">
+      <c r="B85" s="1"/>
+      <c r="D85" s="4"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="1"/>
+      <c r="D86" s="4"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="1"/>
+      <c r="D87" s="4"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88">
+      <c r="B88" s="1"/>
+      <c r="D88" s="4"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89">
+      <c r="B89" s="1"/>
+      <c r="D89" s="4"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90">
+      <c r="B90" s="1"/>
+      <c r="D90" s="4"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91">
+      <c r="B91" s="1"/>
+      <c r="D91" s="4"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92">
+      <c r="B92" s="1"/>
+      <c r="D92" s="4"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93">
+      <c r="B93" s="1"/>
+      <c r="D93" s="4"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94">
+      <c r="B94" s="1"/>
+      <c r="D94" s="4"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95">
+      <c r="B95" s="1"/>
+      <c r="D95" s="4"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96">
+      <c r="B96" s="1"/>
+      <c r="D96" s="4"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="1"/>
+      <c r="D97" s="4"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98">
+      <c r="B98" s="1"/>
+      <c r="D98" s="4"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99">
+      <c r="B99" s="1"/>
+      <c r="D99" s="4"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100">
+      <c r="B100" s="1"/>
+      <c r="D100" s="4"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101">
+      <c r="B101" s="1"/>
+      <c r="D101" s="4"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102">
+      <c r="B102" s="1"/>
+      <c r="D102" s="4"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103">
+      <c r="B103" s="1"/>
+      <c r="D103" s="4"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>